<commit_message>
feat: new data sets for 2019
</commit_message>
<xml_diff>
--- a/data set/State and UT Wise Crimes/State+UT Wise Crime Data of India (IPC) 2001-2018.xlsx
+++ b/data set/State and UT Wise Crimes/State+UT Wise Crime Data of India (IPC) 2001-2018.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayank\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mayank\Repositories\Crime-Prediction-Analysis\data set\State and UT Wise Crimes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE123B7-FD4A-41EB-ABB4-49B899B203D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EA243B-D6DB-44F1-94DC-BB61F46A3B90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="43">
   <si>
     <t>Category</t>
   </si>
@@ -969,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection sqref="A1:H37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1948,10 +1948,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA7AFE0E-371C-40B7-A6F2-1E35B5EE9788}">
-  <dimension ref="A1:F619"/>
+  <dimension ref="A1:F654"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A625" zoomScale="97" workbookViewId="0">
+      <selection activeCell="E654" sqref="E654"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12519,6 +12519,601 @@
         <v>3606</v>
       </c>
     </row>
+    <row r="620" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A620" s="6">
+        <v>1</v>
+      </c>
+      <c r="B620" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C620" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D620" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E620" s="6">
+        <v>237567</v>
+      </c>
+    </row>
+    <row r="621" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A621" s="6">
+        <v>2</v>
+      </c>
+      <c r="B621" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C621" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D621" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E621">
+        <v>2590</v>
+      </c>
+    </row>
+    <row r="622" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A622" s="6">
+        <v>3</v>
+      </c>
+      <c r="B622" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C622" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D622" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E622">
+        <v>123512</v>
+      </c>
+    </row>
+    <row r="623" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A623" s="6">
+        <v>4</v>
+      </c>
+      <c r="B623" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C623" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D623" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E623">
+        <v>197935</v>
+      </c>
+    </row>
+    <row r="624" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A624" s="6">
+        <v>5</v>
+      </c>
+      <c r="B624" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C624" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D624" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E624">
+        <v>61256</v>
+      </c>
+    </row>
+    <row r="625" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A625" s="6">
+        <v>6</v>
+      </c>
+      <c r="B625" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C625" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D625" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E625">
+        <v>2465</v>
+      </c>
+    </row>
+    <row r="626" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A626" s="6">
+        <v>7</v>
+      </c>
+      <c r="B626" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C626" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D626" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E626">
+        <v>139503</v>
+      </c>
+    </row>
+    <row r="627" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A627" s="6">
+        <v>8</v>
+      </c>
+      <c r="B627" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C627" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D627" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E627">
+        <v>111323</v>
+      </c>
+    </row>
+    <row r="628" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A628" s="6">
+        <v>9</v>
+      </c>
+      <c r="B628" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C628" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D628" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E628">
+        <v>14480</v>
+      </c>
+    </row>
+    <row r="629" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A629" s="6">
+        <v>10</v>
+      </c>
+      <c r="B629" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C629" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D629" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E629">
+        <v>22404</v>
+      </c>
+    </row>
+    <row r="630" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A630" s="6">
+        <v>11</v>
+      </c>
+      <c r="B630" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C630" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D630" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E630">
+        <v>50048</v>
+      </c>
+    </row>
+    <row r="631" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A631" s="6">
+        <v>12</v>
+      </c>
+      <c r="B631" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C631" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D631" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E631">
+        <v>120165</v>
+      </c>
+    </row>
+    <row r="632" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A632" s="6">
+        <v>13</v>
+      </c>
+      <c r="B632" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C632" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D632" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E632">
+        <v>175810</v>
+      </c>
+    </row>
+    <row r="633" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A633" s="6">
+        <v>14</v>
+      </c>
+      <c r="B633" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C633" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D633" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E633">
+        <v>246470</v>
+      </c>
+    </row>
+    <row r="634" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A634" s="6">
+        <v>15</v>
+      </c>
+      <c r="B634" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C634" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D634" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E634">
+        <v>341084</v>
+      </c>
+    </row>
+    <row r="635" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A635" s="6">
+        <v>16</v>
+      </c>
+      <c r="B635" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C635" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D635" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E635">
+        <v>2830</v>
+      </c>
+    </row>
+    <row r="636" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A636" s="6">
+        <v>17</v>
+      </c>
+      <c r="B636" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C636" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D636" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E636">
+        <v>3125</v>
+      </c>
+    </row>
+    <row r="637" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A637" s="6">
+        <v>18</v>
+      </c>
+      <c r="B637" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C637" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D637" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E637">
+        <v>2379</v>
+      </c>
+    </row>
+    <row r="638" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A638" s="6">
+        <v>19</v>
+      </c>
+      <c r="B638" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C638" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D638" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E638">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="639" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A639" s="6">
+        <v>20</v>
+      </c>
+      <c r="B639" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C639" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D639" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E639">
+        <v>96033</v>
+      </c>
+    </row>
+    <row r="640" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A640" s="6">
+        <v>21</v>
+      </c>
+      <c r="B640" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C640" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D640" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E640">
+        <v>44697</v>
+      </c>
+    </row>
+    <row r="641" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A641" s="6">
+        <v>22</v>
+      </c>
+      <c r="B641" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C641" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D641" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E641">
+        <v>225306</v>
+      </c>
+    </row>
+    <row r="642" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A642" s="6">
+        <v>23</v>
+      </c>
+      <c r="B642" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C642" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D642" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E642">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="643" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A643" s="6">
+        <v>24</v>
+      </c>
+      <c r="B643" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C643" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D643" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E643">
+        <v>168116</v>
+      </c>
+    </row>
+    <row r="644" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A644" s="6">
+        <v>25</v>
+      </c>
+      <c r="B644" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C644" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D644" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E644">
+        <v>5336</v>
+      </c>
+    </row>
+    <row r="645" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A645" s="6">
+        <v>26</v>
+      </c>
+      <c r="B645" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C645" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D645" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E645">
+        <v>353131</v>
+      </c>
+    </row>
+    <row r="646" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A646" s="6">
+        <v>27</v>
+      </c>
+      <c r="B646" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C646" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D646" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E646">
+        <v>12081</v>
+      </c>
+    </row>
+    <row r="647" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A647" s="6">
+        <v>28</v>
+      </c>
+      <c r="B647" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C647" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D647" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E647">
+        <v>157610</v>
+      </c>
+    </row>
+    <row r="648" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A648" s="6">
+        <v>29</v>
+      </c>
+      <c r="B648" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C648" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D648" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E648">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="649" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A649" s="6">
+        <v>30</v>
+      </c>
+      <c r="B649" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C649" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D649" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E649">
+        <v>2819</v>
+      </c>
+    </row>
+    <row r="650" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A650" s="6">
+        <v>31</v>
+      </c>
+      <c r="B650" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C650" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D650" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E650">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="651" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A651" s="6">
+        <v>32</v>
+      </c>
+      <c r="B651" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C651" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D651" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E651">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="652" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A652" s="6">
+        <v>33</v>
+      </c>
+      <c r="B652" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C652" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D652" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E652">
+        <v>299475</v>
+      </c>
+    </row>
+    <row r="653" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A653" s="6">
+        <v>34</v>
+      </c>
+      <c r="B653" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C653" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D653" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E653">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="654" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A654" s="6">
+        <v>35</v>
+      </c>
+      <c r="B654" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C654" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D654" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E654">
+        <v>3167</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E619">
     <sortCondition ref="D2"/>

</xml_diff>